<commit_message>
Modified 05/08/2024 02:44:51 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -439,49 +439,45 @@
           <t>First Word</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Column 1</t>
-        </is>
-      </c>
+      <c r="B1" s="1" t="inlineStr"/>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Column 2</t>
+          <t>Nr of points</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Column 3</t>
+          <t>Points</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Column 4</t>
+          <t>%-age</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Column 5</t>
+          <t>Column 6</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Column 6</t>
+          <t>Column 7</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Column 7</t>
+          <t>Column 8</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Column 8</t>
+          <t>Column 9</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Column 9</t>
+          <t>Column 10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified 05/08/2024 02:52:14 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -439,47 +439,47 @@
           <t>First Word</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Default green</t>
+        </is>
+      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Nr of points</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Points</t>
+          <t>Yellow</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>%-age</t>
+          <t>Orange</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Column 6</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Column 7</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Column 8</t>
+          <t>Default Red</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Column 9</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Column 10</t>
-        </is>
-      </c>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">

</xml_diff>

<commit_message>
Modified 05/08/2024 03:00:18 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>First Word</t>
+          <t>Car Names</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -479,7 +479,11 @@
           <t>Blue</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr"/>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Predicted headform score (excluding blue points)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">

</xml_diff>

<commit_message>
Modified 05/08/2024 03:14:08 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -432,6 +432,18 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.2" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="8.4" customWidth="1" min="3" max="3"/>
+    <col width="9.6" customWidth="1" min="4" max="4"/>
+    <col width="9.6" customWidth="1" min="5" max="5"/>
+    <col width="8.4" customWidth="1" min="6" max="6"/>
+    <col width="6" customWidth="1" min="7" max="7"/>
+    <col width="15.6" customWidth="1" min="8" max="8"/>
+    <col width="7.199999999999999" customWidth="1" min="9" max="9"/>
+    <col width="60" customWidth="1" min="10" max="10"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -492,31 +504,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1168831168831169</v>
+        <v>11.69</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3441558441558442</v>
+        <v>34.42</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2727272727272727</v>
+        <v>27.27</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09740259740259741</v>
+        <v>9.74</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02597402597402598</v>
+        <v>2.6</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07792207792207792</v>
+        <v>7.79</v>
       </c>
       <c r="H2" t="n">
-        <v>0.06493506493506493</v>
+        <v>6.49</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -529,19 +541,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4698795180722892</v>
+        <v>46.99</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3674698795180723</v>
+        <v>36.75</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05421686746987952</v>
+        <v>5.42</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07228915662650602</v>
+        <v>7.23</v>
       </c>
       <c r="G3" t="n">
-        <v>0.03614457831325301</v>
+        <v>3.61</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -550,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -560,31 +572,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1730769230769231</v>
+        <v>17.31</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2307692307692308</v>
+        <v>23.08</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2564102564102564</v>
+        <v>25.64</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1217948717948718</v>
+        <v>12.18</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0576923076923077</v>
+        <v>5.77</v>
       </c>
       <c r="G4" t="n">
-        <v>0.08333333333333333</v>
+        <v>8.33</v>
       </c>
       <c r="H4" t="n">
-        <v>0.07692307692307693</v>
+        <v>7.69</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -597,19 +609,19 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4968152866242038</v>
+        <v>49.68</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1719745222929936</v>
+        <v>17.2</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2229299363057325</v>
+        <v>22.29</v>
       </c>
       <c r="F5" t="n">
-        <v>0.06369426751592357</v>
+        <v>6.37</v>
       </c>
       <c r="G5" t="n">
-        <v>0.04458598726114649</v>
+        <v>4.46</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -618,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
@@ -631,28 +643,28 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2951807228915663</v>
+        <v>29.52</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2469879518072289</v>
+        <v>24.7</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1927710843373494</v>
+        <v>19.28</v>
       </c>
       <c r="F6" t="n">
-        <v>0.09036144578313253</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1385542168674699</v>
+        <v>13.86</v>
       </c>
       <c r="H6" t="n">
-        <v>0.03614457831325301</v>
+        <v>3.61</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
@@ -665,28 +677,28 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2252747252747253</v>
+        <v>22.53</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3626373626373626</v>
+        <v>36.26</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1648351648351648</v>
+        <v>16.48</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0989010989010989</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1263736263736264</v>
+        <v>12.64</v>
       </c>
       <c r="H7" t="n">
-        <v>0.02197802197802198</v>
+        <v>2.2</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
@@ -696,31 +708,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1513157894736842</v>
+        <v>15.13</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3684210526315789</v>
+        <v>36.84</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1973684210526316</v>
+        <v>19.74</v>
       </c>
       <c r="E8" t="n">
-        <v>0.09868421052631579</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03947368421052631</v>
+        <v>3.95</v>
       </c>
       <c r="G8" t="n">
-        <v>0.09210526315789473</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>0.05263157894736842</v>
+        <v>5.26</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9">
@@ -730,31 +742,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2098765432098765</v>
+        <v>20.99</v>
       </c>
       <c r="C9" t="n">
-        <v>0.08024691358024691</v>
+        <v>8.02</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2037037037037037</v>
+        <v>20.37</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2222222222222222</v>
+        <v>22.22</v>
       </c>
       <c r="F9" t="n">
-        <v>0.08641975308641975</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1234567901234568</v>
+        <v>12.35</v>
       </c>
       <c r="H9" t="n">
-        <v>0.07407407407407407</v>
+        <v>7.41</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
@@ -767,19 +779,19 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1419753086419753</v>
+        <v>14.2</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5185185185185185</v>
+        <v>51.85</v>
       </c>
       <c r="E10" t="n">
-        <v>0.228395061728395</v>
+        <v>22.84</v>
       </c>
       <c r="F10" t="n">
-        <v>0.08641975308641975</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="G10" t="n">
-        <v>0.02469135802469136</v>
+        <v>2.47</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -788,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0.9999999999999999</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -798,31 +810,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.01807228915662651</v>
+        <v>1.81</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2228915662650602</v>
+        <v>22.29</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2530120481927711</v>
+        <v>25.3</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2168674698795181</v>
+        <v>21.69</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1265060240963855</v>
+        <v>12.65</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1265060240963855</v>
+        <v>12.65</v>
       </c>
       <c r="H11" t="n">
-        <v>0.03614457831325301</v>
+        <v>3.61</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified 05/08/2024 03:42:59 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -433,16 +433,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.2" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="8.4" customWidth="1" min="3" max="3"/>
-    <col width="9.6" customWidth="1" min="4" max="4"/>
-    <col width="9.6" customWidth="1" min="5" max="5"/>
-    <col width="8.4" customWidth="1" min="6" max="6"/>
-    <col width="6" customWidth="1" min="7" max="7"/>
-    <col width="15.6" customWidth="1" min="8" max="8"/>
-    <col width="7.199999999999999" customWidth="1" min="9" max="9"/>
-    <col width="60" customWidth="1" min="10" max="10"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="7" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
+    <col width="5" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="6" customWidth="1" min="9" max="9"/>
+    <col width="50" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Modified 05/08/2024 04:04:33 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -500,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Toyota_Yaris_2020_</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -534,7 +534,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mazda</t>
+          <t>Mazda_MX-30_2020_</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -568,7 +568,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Honda_Jazz_2020_</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -602,7 +602,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Land</t>
+          <t xml:space="preserve">Landrover Defender </t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -636,7 +636,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SEAT</t>
+          <t>SEAT_Leon_2020_</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -670,7 +670,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>KIA</t>
+          <t>Kia_Sorento_2020_</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -704,7 +704,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t xml:space="preserve">Honda e </t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -738,7 +738,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Hyundai_i10_2020_</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -772,7 +772,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ISUZU</t>
+          <t>Isuzu_D-Max_2020_</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -806,7 +806,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Audi</t>
+          <t xml:space="preserve">Audi A3 </t>
         </is>
       </c>
       <c r="B11" t="n">

</xml_diff>

<commit_message>
Modified 05/08/2024 04:13:28 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -500,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Toyota_Yaris_2020_</t>
+          <t>Toyota Yaris  2020</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -534,29 +534,29 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mazda_MX-30_2020_</t>
+          <t>Honda Jazz  2020</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>17.31</v>
       </c>
       <c r="C3" t="n">
-        <v>46.99</v>
+        <v>23.08</v>
       </c>
       <c r="D3" t="n">
-        <v>36.75</v>
+        <v>25.64</v>
       </c>
       <c r="E3" t="n">
-        <v>5.42</v>
+        <v>12.18</v>
       </c>
       <c r="F3" t="n">
-        <v>7.23</v>
+        <v>5.77</v>
       </c>
       <c r="G3" t="n">
-        <v>3.61</v>
+        <v>8.33</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>7.69</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -568,29 +568,29 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Honda_Jazz_2020_</t>
+          <t>SEAT Leon  2020</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17.31</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>23.08</v>
+        <v>29.52</v>
       </c>
       <c r="D4" t="n">
-        <v>25.64</v>
+        <v>24.7</v>
       </c>
       <c r="E4" t="n">
-        <v>12.18</v>
+        <v>19.28</v>
       </c>
       <c r="F4" t="n">
-        <v>5.77</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="G4" t="n">
-        <v>8.33</v>
+        <v>13.86</v>
       </c>
       <c r="H4" t="n">
-        <v>7.69</v>
+        <v>3.61</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -602,29 +602,29 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Landrover Defender </t>
+          <t>Kia Sorento  2020</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>49.68</v>
+        <v>22.53</v>
       </c>
       <c r="D5" t="n">
-        <v>17.2</v>
+        <v>36.26</v>
       </c>
       <c r="E5" t="n">
-        <v>22.29</v>
+        <v>16.48</v>
       </c>
       <c r="F5" t="n">
-        <v>6.37</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>4.46</v>
+        <v>12.64</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -636,204 +636,34 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SEAT_Leon_2020_</t>
+          <t>Isuzu D-Max  2020</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>29.52</v>
+        <v>14.2</v>
       </c>
       <c r="D6" t="n">
-        <v>24.7</v>
+        <v>51.85</v>
       </c>
       <c r="E6" t="n">
-        <v>19.28</v>
+        <v>22.84</v>
       </c>
       <c r="F6" t="n">
-        <v>9.039999999999999</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="G6" t="n">
-        <v>13.86</v>
+        <v>2.47</v>
       </c>
       <c r="H6" t="n">
-        <v>3.61</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Kia_Sorento_2020_</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>22.53</v>
-      </c>
-      <c r="D7" t="n">
-        <v>36.26</v>
-      </c>
-      <c r="E7" t="n">
-        <v>16.48</v>
-      </c>
-      <c r="F7" t="n">
-        <v>9.890000000000001</v>
-      </c>
-      <c r="G7" t="n">
-        <v>12.64</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Honda e </t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>15.13</v>
-      </c>
-      <c r="C8" t="n">
-        <v>36.84</v>
-      </c>
-      <c r="D8" t="n">
-        <v>19.74</v>
-      </c>
-      <c r="E8" t="n">
-        <v>9.869999999999999</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3.95</v>
-      </c>
-      <c r="G8" t="n">
-        <v>9.210000000000001</v>
-      </c>
-      <c r="H8" t="n">
-        <v>5.26</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Hyundai_i10_2020_</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>20.99</v>
-      </c>
-      <c r="C9" t="n">
-        <v>8.02</v>
-      </c>
-      <c r="D9" t="n">
-        <v>20.37</v>
-      </c>
-      <c r="E9" t="n">
-        <v>22.22</v>
-      </c>
-      <c r="F9" t="n">
-        <v>8.640000000000001</v>
-      </c>
-      <c r="G9" t="n">
-        <v>12.35</v>
-      </c>
-      <c r="H9" t="n">
-        <v>7.41</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Isuzu_D-Max_2020_</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>14.2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>51.85</v>
-      </c>
-      <c r="E10" t="n">
-        <v>22.84</v>
-      </c>
-      <c r="F10" t="n">
-        <v>8.640000000000001</v>
-      </c>
-      <c r="G10" t="n">
-        <v>2.47</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Audi A3 </t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1.81</v>
-      </c>
-      <c r="C11" t="n">
-        <v>22.29</v>
-      </c>
-      <c r="D11" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="E11" t="n">
-        <v>21.69</v>
-      </c>
-      <c r="F11" t="n">
-        <v>12.65</v>
-      </c>
-      <c r="G11" t="n">
-        <v>12.65</v>
-      </c>
-      <c r="H11" t="n">
-        <v>3.61</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified 05/08/2024 04:36:11 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -500,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Toyota Yaris  2020</t>
+          <t xml:space="preserve">Toyota Yaris 2020 </t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -534,29 +534,29 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Honda Jazz  2020</t>
+          <t xml:space="preserve">Mazda MX 30 2020 </t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17.31</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>23.08</v>
+        <v>46.99</v>
       </c>
       <c r="D3" t="n">
-        <v>25.64</v>
+        <v>36.75</v>
       </c>
       <c r="E3" t="n">
-        <v>12.18</v>
+        <v>5.42</v>
       </c>
       <c r="F3" t="n">
-        <v>5.77</v>
+        <v>7.23</v>
       </c>
       <c r="G3" t="n">
-        <v>8.33</v>
+        <v>3.61</v>
       </c>
       <c r="H3" t="n">
-        <v>7.69</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -568,29 +568,29 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SEAT Leon  2020</t>
+          <t xml:space="preserve">Honda Jazz 2020 </t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>17.31</v>
       </c>
       <c r="C4" t="n">
-        <v>29.52</v>
+        <v>23.08</v>
       </c>
       <c r="D4" t="n">
-        <v>24.7</v>
+        <v>25.64</v>
       </c>
       <c r="E4" t="n">
-        <v>19.28</v>
+        <v>12.18</v>
       </c>
       <c r="F4" t="n">
-        <v>9.039999999999999</v>
+        <v>5.77</v>
       </c>
       <c r="G4" t="n">
-        <v>13.86</v>
+        <v>8.33</v>
       </c>
       <c r="H4" t="n">
-        <v>3.61</v>
+        <v>7.69</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -602,29 +602,29 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kia Sorento  2020</t>
+          <t xml:space="preserve">Landrover Defender </t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>22.53</v>
+        <v>49.68</v>
       </c>
       <c r="D5" t="n">
-        <v>36.26</v>
+        <v>17.2</v>
       </c>
       <c r="E5" t="n">
-        <v>16.48</v>
+        <v>22.29</v>
       </c>
       <c r="F5" t="n">
-        <v>9.890000000000001</v>
+        <v>6.37</v>
       </c>
       <c r="G5" t="n">
-        <v>12.64</v>
+        <v>4.46</v>
       </c>
       <c r="H5" t="n">
-        <v>2.2</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -636,34 +636,204 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Isuzu D-Max  2020</t>
+          <t xml:space="preserve">SEAT Leon 2020 </t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
+        <v>29.52</v>
+      </c>
+      <c r="D6" t="n">
+        <v>24.7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>19.28</v>
+      </c>
+      <c r="F6" t="n">
+        <v>9.039999999999999</v>
+      </c>
+      <c r="G6" t="n">
+        <v>13.86</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kia Sorento 2020 </t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>22.53</v>
+      </c>
+      <c r="D7" t="n">
+        <v>36.26</v>
+      </c>
+      <c r="E7" t="n">
+        <v>16.48</v>
+      </c>
+      <c r="F7" t="n">
+        <v>9.890000000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>12.64</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honda e </t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>15.13</v>
+      </c>
+      <c r="C8" t="n">
+        <v>36.84</v>
+      </c>
+      <c r="D8" t="n">
+        <v>19.74</v>
+      </c>
+      <c r="E8" t="n">
+        <v>9.869999999999999</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="G8" t="n">
+        <v>9.210000000000001</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hyundai i10 2020 </t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>20.99</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8.02</v>
+      </c>
+      <c r="D9" t="n">
+        <v>20.37</v>
+      </c>
+      <c r="E9" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8.640000000000001</v>
+      </c>
+      <c r="G9" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="H9" t="n">
+        <v>7.41</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Isuzu D Max 2020 </t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
         <v>14.2</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D10" t="n">
         <v>51.85</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E10" t="n">
         <v>22.84</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F10" t="n">
         <v>8.640000000000001</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G10" t="n">
         <v>2.47</v>
       </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Audi A3 </t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="C11" t="n">
+        <v>22.29</v>
+      </c>
+      <c r="D11" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="E11" t="n">
+        <v>21.69</v>
+      </c>
+      <c r="F11" t="n">
+        <v>12.65</v>
+      </c>
+      <c r="G11" t="n">
+        <v>12.65</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified 05/08/2024 05:13:39 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -500,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Toyota Yaris 2020 </t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -534,7 +534,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mazda MX 30 2020 </t>
+          <t>Mazda</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -568,7 +568,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Honda Jazz 2020 </t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -602,7 +602,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Landrover Defender </t>
+          <t>Land</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -636,7 +636,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">SEAT Leon 2020 </t>
+          <t>SEAT</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -670,7 +670,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kia Sorento 2020 </t>
+          <t>KIA</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -704,7 +704,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Honda e </t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -738,7 +738,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hyundai i10 2020 </t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -772,7 +772,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Isuzu D Max 2020 </t>
+          <t>ISUZU</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -806,7 +806,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Audi A3 </t>
+          <t>Audi</t>
         </is>
       </c>
       <c r="B11" t="n">

</xml_diff>

<commit_message>
Modified 05/08/2024 05:21:06 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -500,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Toyota Yaris</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -534,7 +534,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mazda</t>
+          <t>Mazda MX-30</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -568,7 +568,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Honda JAZZ</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -602,7 +602,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Land</t>
+          <t>Land Rover Defender</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -636,7 +636,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SEAT</t>
+          <t>SEAT Leon</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -670,7 +670,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>KIA</t>
+          <t>KIA Sorento</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -704,7 +704,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Honda e</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -738,7 +738,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Hyundai i10</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -772,7 +772,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ISUZU</t>
+          <t>ISUZU D-Max Crew Cab</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -806,7 +806,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Audi</t>
+          <t>Audi A3</t>
         </is>
       </c>
       <c r="B11" t="n">

</xml_diff>

<commit_message>
Modified 06/08/2024 11:52:56 AM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Graphs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -134,6 +135,236 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>26</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>26</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>52</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>52</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>78</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>78</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>104</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6000750" cy="4476750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -840,4 +1071,29 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K105"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1"/>
+    <row r="27"/>
+    <row r="53"/>
+    <row r="79"/>
+    <row r="105"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified 06/08/2024 12:55:30 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (C) - Color-wise data/2020_cars_combined.xlsx
@@ -735,25 +735,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11.69</v>
+        <v>11.68831168831169</v>
       </c>
       <c r="C2" t="n">
-        <v>34.42</v>
+        <v>34.41558441558442</v>
       </c>
       <c r="D2" t="n">
-        <v>27.27</v>
+        <v>27.27272727272727</v>
       </c>
       <c r="E2" t="n">
-        <v>9.74</v>
+        <v>9.740259740259742</v>
       </c>
       <c r="F2" t="n">
-        <v>2.6</v>
+        <v>2.597402597402597</v>
       </c>
       <c r="G2" t="n">
-        <v>7.79</v>
+        <v>7.792207792207792</v>
       </c>
       <c r="H2" t="n">
-        <v>6.49</v>
+        <v>6.493506493506493</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -772,19 +772,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>46.99</v>
+        <v>46.98795180722892</v>
       </c>
       <c r="D3" t="n">
-        <v>36.75</v>
+        <v>36.74698795180723</v>
       </c>
       <c r="E3" t="n">
-        <v>5.42</v>
+        <v>5.421686746987952</v>
       </c>
       <c r="F3" t="n">
-        <v>7.23</v>
+        <v>7.228915662650602</v>
       </c>
       <c r="G3" t="n">
-        <v>3.61</v>
+        <v>3.614457831325301</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -803,25 +803,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17.31</v>
+        <v>17.30769230769231</v>
       </c>
       <c r="C4" t="n">
-        <v>23.08</v>
+        <v>23.07692307692308</v>
       </c>
       <c r="D4" t="n">
-        <v>25.64</v>
+        <v>25.64102564102564</v>
       </c>
       <c r="E4" t="n">
-        <v>12.18</v>
+        <v>12.17948717948718</v>
       </c>
       <c r="F4" t="n">
-        <v>5.77</v>
+        <v>5.769230769230769</v>
       </c>
       <c r="G4" t="n">
-        <v>8.33</v>
+        <v>8.333333333333332</v>
       </c>
       <c r="H4" t="n">
-        <v>7.69</v>
+        <v>7.692307692307693</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -840,19 +840,19 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>49.68</v>
+        <v>49.68152866242038</v>
       </c>
       <c r="D5" t="n">
-        <v>17.2</v>
+        <v>17.19745222929936</v>
       </c>
       <c r="E5" t="n">
-        <v>22.29</v>
+        <v>22.29299363057325</v>
       </c>
       <c r="F5" t="n">
-        <v>6.37</v>
+        <v>6.369426751592357</v>
       </c>
       <c r="G5" t="n">
-        <v>4.46</v>
+        <v>4.45859872611465</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -874,22 +874,22 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>29.52</v>
+        <v>29.51807228915663</v>
       </c>
       <c r="D6" t="n">
-        <v>24.7</v>
+        <v>24.69879518072289</v>
       </c>
       <c r="E6" t="n">
-        <v>19.28</v>
+        <v>19.27710843373494</v>
       </c>
       <c r="F6" t="n">
-        <v>9.039999999999999</v>
+        <v>9.036144578313253</v>
       </c>
       <c r="G6" t="n">
-        <v>13.86</v>
+        <v>13.85542168674699</v>
       </c>
       <c r="H6" t="n">
-        <v>3.61</v>
+        <v>3.614457831325301</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -908,22 +908,22 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>22.53</v>
+        <v>22.52747252747253</v>
       </c>
       <c r="D7" t="n">
-        <v>36.26</v>
+        <v>36.26373626373626</v>
       </c>
       <c r="E7" t="n">
-        <v>16.48</v>
+        <v>16.48351648351648</v>
       </c>
       <c r="F7" t="n">
-        <v>9.890000000000001</v>
+        <v>9.890109890109891</v>
       </c>
       <c r="G7" t="n">
-        <v>12.64</v>
+        <v>12.63736263736264</v>
       </c>
       <c r="H7" t="n">
-        <v>2.2</v>
+        <v>2.197802197802198</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -939,25 +939,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>15.13</v>
+        <v>15.13157894736842</v>
       </c>
       <c r="C8" t="n">
-        <v>36.84</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="D8" t="n">
-        <v>19.74</v>
+        <v>19.73684210526316</v>
       </c>
       <c r="E8" t="n">
-        <v>9.869999999999999</v>
+        <v>9.868421052631579</v>
       </c>
       <c r="F8" t="n">
-        <v>3.95</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="G8" t="n">
-        <v>9.210000000000001</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="H8" t="n">
-        <v>5.26</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -973,25 +973,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20.99</v>
+        <v>20.98765432098765</v>
       </c>
       <c r="C9" t="n">
-        <v>8.02</v>
+        <v>8.024691358024691</v>
       </c>
       <c r="D9" t="n">
-        <v>20.37</v>
+        <v>20.37037037037037</v>
       </c>
       <c r="E9" t="n">
-        <v>22.22</v>
+        <v>22.22222222222222</v>
       </c>
       <c r="F9" t="n">
-        <v>8.640000000000001</v>
+        <v>8.641975308641975</v>
       </c>
       <c r="G9" t="n">
-        <v>12.35</v>
+        <v>12.34567901234568</v>
       </c>
       <c r="H9" t="n">
-        <v>7.41</v>
+        <v>7.407407407407407</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -1010,19 +1010,19 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>14.2</v>
+        <v>14.19753086419753</v>
       </c>
       <c r="D10" t="n">
-        <v>51.85</v>
+        <v>51.85185185185185</v>
       </c>
       <c r="E10" t="n">
-        <v>22.84</v>
+        <v>22.83950617283951</v>
       </c>
       <c r="F10" t="n">
-        <v>8.640000000000001</v>
+        <v>8.641975308641975</v>
       </c>
       <c r="G10" t="n">
-        <v>2.47</v>
+        <v>2.469135802469136</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1031,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>100</v>
+        <v>99.99999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -1041,25 +1041,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.81</v>
+        <v>1.80722891566265</v>
       </c>
       <c r="C11" t="n">
-        <v>22.29</v>
+        <v>22.28915662650602</v>
       </c>
       <c r="D11" t="n">
-        <v>25.3</v>
+        <v>25.30120481927711</v>
       </c>
       <c r="E11" t="n">
-        <v>21.69</v>
+        <v>21.68674698795181</v>
       </c>
       <c r="F11" t="n">
-        <v>12.65</v>
+        <v>12.65060240963855</v>
       </c>
       <c r="G11" t="n">
-        <v>12.65</v>
+        <v>12.65060240963855</v>
       </c>
       <c r="H11" t="n">
-        <v>3.61</v>
+        <v>3.614457831325301</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>

</xml_diff>